<commit_message>
bj: update cov survey for benin
</commit_message>
<xml_diff>
--- a/Coverage Survey/Benin/bj_sct_lf_1_cov_202406.xlsx
+++ b/Coverage Survey/Benin/bj_sct_lf_1_cov_202406.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\Coverage Survey\Benin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431D5DAF-7ADF-4543-B85B-C6540E9374D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E05BDAA-D470-463A-81CE-A13127EA00D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1685" uniqueCount="580">
   <si>
     <t>type</t>
   </si>
@@ -1770,6 +1770,12 @@
   </si>
   <si>
     <t>Q43. Quel est le résultat du test à la bandelette à la bandelette urinaire</t>
+  </si>
+  <si>
+    <t>Trace non hémolysée</t>
+  </si>
+  <si>
+    <t>Trace.non.hémolysée</t>
   </si>
 </sst>
 </file>
@@ -2383,9 +2389,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C82" sqref="C82"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75"/>
@@ -3584,6 +3590,9 @@
       <c r="E66" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="H66" s="5" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="67" spans="1:12">
       <c r="A67" s="5" t="s">
@@ -3861,6 +3870,9 @@
       <c r="C83" s="5" t="s">
         <v>26</v>
       </c>
+      <c r="H83" s="5" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="84" spans="1:8">
       <c r="A84" s="5" t="s">
@@ -3891,11 +3903,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G359"/>
+  <dimension ref="A1:G360"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B88" sqref="B88"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A193" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C241" sqref="C241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75"/>
@@ -7346,10 +7358,10 @@
         <v>323</v>
       </c>
       <c r="B241" s="19" t="s">
-        <v>328</v>
+        <v>579</v>
       </c>
       <c r="C241" s="19" t="s">
-        <v>328</v>
+        <v>578</v>
       </c>
       <c r="D241" s="15"/>
       <c r="E241" s="16"/>
@@ -7361,10 +7373,10 @@
         <v>323</v>
       </c>
       <c r="B242" s="19" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C242" s="19" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D242" s="15"/>
       <c r="E242" s="16"/>
@@ -7376,10 +7388,10 @@
         <v>323</v>
       </c>
       <c r="B243" s="19" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C243" s="19" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D243" s="15"/>
       <c r="E243" s="16"/>
@@ -7387,34 +7399,38 @@
       <c r="G243" s="16"/>
     </row>
     <row r="244" spans="1:7">
-      <c r="A244" s="19"/>
-      <c r="B244" s="19"/>
-      <c r="C244" s="19"/>
+      <c r="A244" s="19" t="s">
+        <v>323</v>
+      </c>
+      <c r="B244" s="19" t="s">
+        <v>330</v>
+      </c>
+      <c r="C244" s="19" t="s">
+        <v>330</v>
+      </c>
       <c r="D244" s="15"/>
       <c r="E244" s="16"/>
       <c r="F244" s="16"/>
       <c r="G244" s="16"/>
     </row>
     <row r="245" spans="1:7">
-      <c r="A245" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B245" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C245" s="5" t="s">
-        <v>56</v>
-      </c>
+      <c r="A245" s="19"/>
+      <c r="B245" s="19"/>
+      <c r="C245" s="19"/>
+      <c r="D245" s="15"/>
+      <c r="E245" s="16"/>
+      <c r="F245" s="16"/>
+      <c r="G245" s="16"/>
     </row>
     <row r="246" spans="1:7">
       <c r="A246" s="5" t="s">
         <v>107</v>
       </c>
       <c r="B246" s="5" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C246" s="5" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="247" spans="1:7">
@@ -7422,10 +7438,10 @@
         <v>107</v>
       </c>
       <c r="B247" s="5" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C247" s="5" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="248" spans="1:7">
@@ -7433,10 +7449,10 @@
         <v>107</v>
       </c>
       <c r="B248" s="5" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="C248" s="5" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
     <row r="249" spans="1:7">
@@ -7444,10 +7460,10 @@
         <v>107</v>
       </c>
       <c r="B249" s="5" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="C249" s="5" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
     </row>
     <row r="250" spans="1:7">
@@ -7455,10 +7471,10 @@
         <v>107</v>
       </c>
       <c r="B250" s="5" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C250" s="5" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
     </row>
     <row r="251" spans="1:7">
@@ -7466,24 +7482,21 @@
         <v>107</v>
       </c>
       <c r="B251" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C251" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7">
+      <c r="A252" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B252" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C251" s="5" t="s">
+      <c r="C252" s="5" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="253" spans="1:7">
-      <c r="A253" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B253" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C253" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D253" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="254" spans="1:7">
@@ -7491,10 +7504,10 @@
         <v>108</v>
       </c>
       <c r="B254" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C254" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D254" s="5" t="s">
         <v>56</v>
@@ -7505,10 +7518,10 @@
         <v>108</v>
       </c>
       <c r="B255" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C255" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D255" s="5" t="s">
         <v>56</v>
@@ -7519,13 +7532,13 @@
         <v>108</v>
       </c>
       <c r="B256" s="5" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C256" s="5" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="D256" s="5" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="257" spans="1:5">
@@ -7533,13 +7546,13 @@
         <v>108</v>
       </c>
       <c r="B257" s="5" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C257" s="5" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="D257" s="5" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="258" spans="1:5">
@@ -7547,10 +7560,10 @@
         <v>108</v>
       </c>
       <c r="B258" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C258" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D258" s="5" t="s">
         <v>60</v>
@@ -7561,10 +7574,10 @@
         <v>108</v>
       </c>
       <c r="B259" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C259" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D259" s="5" t="s">
         <v>60</v>
@@ -7575,13 +7588,13 @@
         <v>108</v>
       </c>
       <c r="B260" s="5" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="C260" s="5" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="D260" s="5" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
     <row r="261" spans="1:5">
@@ -7589,10 +7602,10 @@
         <v>108</v>
       </c>
       <c r="B261" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C261" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D261" s="5" t="s">
         <v>49</v>
@@ -7603,13 +7616,13 @@
         <v>108</v>
       </c>
       <c r="B262" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C262" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D262" s="5" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
     </row>
     <row r="263" spans="1:5">
@@ -7617,13 +7630,13 @@
         <v>108</v>
       </c>
       <c r="B263" s="5" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C263" s="5" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D263" s="5" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
     </row>
     <row r="264" spans="1:5">
@@ -7631,10 +7644,10 @@
         <v>108</v>
       </c>
       <c r="B264" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C264" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D264" s="5" t="s">
         <v>44</v>
@@ -7645,10 +7658,10 @@
         <v>108</v>
       </c>
       <c r="B265" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C265" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D265" s="5" t="s">
         <v>44</v>
@@ -7659,13 +7672,13 @@
         <v>108</v>
       </c>
       <c r="B266" s="5" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C266" s="5" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D266" s="5" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="267" spans="1:5">
@@ -7673,27 +7686,27 @@
         <v>108</v>
       </c>
       <c r="B267" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C267" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D267" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="269" spans="1:5">
-      <c r="A269" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B269" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C269" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E269" s="5" t="s">
-        <v>45</v>
+    <row r="268" spans="1:5">
+      <c r="A268" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B268" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C268" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D268" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="270" spans="1:5">
@@ -7701,10 +7714,10 @@
         <v>111</v>
       </c>
       <c r="B270" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C270" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E270" s="5" t="s">
         <v>45</v>
@@ -7715,10 +7728,10 @@
         <v>111</v>
       </c>
       <c r="B271" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C271" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E271" s="5" t="s">
         <v>45</v>
@@ -7729,13 +7742,13 @@
         <v>111</v>
       </c>
       <c r="B272" s="5" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="C272" s="5" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="E272" s="5" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="273" spans="1:5">
@@ -7743,10 +7756,10 @@
         <v>111</v>
       </c>
       <c r="B273" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C273" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E273" s="5" t="s">
         <v>57</v>
@@ -7757,10 +7770,10 @@
         <v>111</v>
       </c>
       <c r="B274" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C274" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E274" s="5" t="s">
         <v>57</v>
@@ -7771,13 +7784,13 @@
         <v>111</v>
       </c>
       <c r="B275" s="5" t="s">
-        <v>52</v>
+        <v>89</v>
       </c>
       <c r="C275" s="5" t="s">
-        <v>52</v>
+        <v>89</v>
       </c>
       <c r="E275" s="5" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="276" spans="1:5">
@@ -7785,10 +7798,10 @@
         <v>111</v>
       </c>
       <c r="B276" s="5" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="C276" s="5" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="E276" s="5" t="s">
         <v>52</v>
@@ -7799,10 +7812,10 @@
         <v>111</v>
       </c>
       <c r="B277" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C277" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E277" s="5" t="s">
         <v>52</v>
@@ -7813,13 +7826,13 @@
         <v>111</v>
       </c>
       <c r="B278" s="5" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C278" s="5" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="E278" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="279" spans="1:5">
@@ -7827,10 +7840,10 @@
         <v>111</v>
       </c>
       <c r="B279" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C279" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E279" s="5" t="s">
         <v>48</v>
@@ -7841,10 +7854,10 @@
         <v>111</v>
       </c>
       <c r="B280" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C280" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E280" s="5" t="s">
         <v>48</v>
@@ -7855,13 +7868,13 @@
         <v>111</v>
       </c>
       <c r="B281" s="5" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="C281" s="5" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="E281" s="5" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="282" spans="1:5">
@@ -7869,10 +7882,10 @@
         <v>111</v>
       </c>
       <c r="B282" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C282" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E282" s="5" t="s">
         <v>61</v>
@@ -7883,10 +7896,10 @@
         <v>111</v>
       </c>
       <c r="B283" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C283" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E283" s="5" t="s">
         <v>61</v>
@@ -7897,13 +7910,13 @@
         <v>111</v>
       </c>
       <c r="B284" s="5" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="C284" s="5" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="E284" s="5" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
     <row r="285" spans="1:5">
@@ -7911,10 +7924,10 @@
         <v>111</v>
       </c>
       <c r="B285" s="5" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="C285" s="5" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="E285" s="5" t="s">
         <v>50</v>
@@ -7925,10 +7938,10 @@
         <v>111</v>
       </c>
       <c r="B286" s="5" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="C286" s="5" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="E286" s="5" t="s">
         <v>50</v>
@@ -7939,13 +7952,13 @@
         <v>111</v>
       </c>
       <c r="B287" s="5" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C287" s="5" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E287" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="288" spans="1:5">
@@ -7953,10 +7966,10 @@
         <v>111</v>
       </c>
       <c r="B288" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C288" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E288" s="5" t="s">
         <v>54</v>
@@ -7967,10 +7980,10 @@
         <v>111</v>
       </c>
       <c r="B289" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C289" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E289" s="5" t="s">
         <v>54</v>
@@ -7981,13 +7994,13 @@
         <v>111</v>
       </c>
       <c r="B290" s="5" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="C290" s="5" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="E290" s="5" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="291" spans="1:5">
@@ -7995,10 +8008,10 @@
         <v>111</v>
       </c>
       <c r="B291" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C291" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E291" s="5" t="s">
         <v>46</v>
@@ -8009,10 +8022,10 @@
         <v>111</v>
       </c>
       <c r="B292" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C292" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E292" s="5" t="s">
         <v>46</v>
@@ -8023,13 +8036,13 @@
         <v>111</v>
       </c>
       <c r="B293" s="5" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="C293" s="5" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="E293" s="5" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="294" spans="1:5">
@@ -8037,10 +8050,10 @@
         <v>111</v>
       </c>
       <c r="B294" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C294" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E294" s="5" t="s">
         <v>58</v>
@@ -8051,10 +8064,10 @@
         <v>111</v>
       </c>
       <c r="B295" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C295" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E295" s="5" t="s">
         <v>58</v>
@@ -8065,13 +8078,13 @@
         <v>111</v>
       </c>
       <c r="B296" s="5" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C296" s="5" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E296" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="297" spans="1:5">
@@ -8079,10 +8092,10 @@
         <v>111</v>
       </c>
       <c r="B297" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C297" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E297" s="5" t="s">
         <v>62</v>
@@ -8093,10 +8106,10 @@
         <v>111</v>
       </c>
       <c r="B298" s="5" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="C298" s="5" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="E298" s="5" t="s">
         <v>62</v>
@@ -8107,13 +8120,13 @@
         <v>111</v>
       </c>
       <c r="B299" s="5" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="C299" s="5" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="E299" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="300" spans="1:5">
@@ -8121,10 +8134,10 @@
         <v>111</v>
       </c>
       <c r="B300" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C300" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E300" s="5" t="s">
         <v>63</v>
@@ -8135,10 +8148,10 @@
         <v>111</v>
       </c>
       <c r="B301" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C301" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E301" s="5" t="s">
         <v>63</v>
@@ -8149,13 +8162,13 @@
         <v>111</v>
       </c>
       <c r="B302" s="5" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="C302" s="5" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="E302" s="5" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
     </row>
     <row r="303" spans="1:5">
@@ -8163,10 +8176,10 @@
         <v>111</v>
       </c>
       <c r="B303" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C303" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E303" s="5" t="s">
         <v>51</v>
@@ -8177,10 +8190,10 @@
         <v>111</v>
       </c>
       <c r="B304" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C304" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E304" s="5" t="s">
         <v>51</v>
@@ -8191,13 +8204,13 @@
         <v>111</v>
       </c>
       <c r="B305" s="5" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C305" s="5" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E305" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="306" spans="1:6">
@@ -8205,10 +8218,10 @@
         <v>111</v>
       </c>
       <c r="B306" s="5" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="C306" s="5" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="E306" s="5" t="s">
         <v>55</v>
@@ -8219,10 +8232,10 @@
         <v>111</v>
       </c>
       <c r="B307" s="5" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="C307" s="5" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="E307" s="5" t="s">
         <v>55</v>
@@ -8233,13 +8246,13 @@
         <v>111</v>
       </c>
       <c r="B308" s="5" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="C308" s="5" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="E308" s="5" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
     </row>
     <row r="309" spans="1:6">
@@ -8247,10 +8260,10 @@
         <v>111</v>
       </c>
       <c r="B309" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C309" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E309" s="5" t="s">
         <v>44</v>
@@ -8261,10 +8274,10 @@
         <v>111</v>
       </c>
       <c r="B310" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C310" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E310" s="5" t="s">
         <v>44</v>
@@ -8275,13 +8288,13 @@
         <v>111</v>
       </c>
       <c r="B311" s="5" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="C311" s="5" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="E311" s="5" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
     <row r="312" spans="1:6">
@@ -8289,10 +8302,10 @@
         <v>111</v>
       </c>
       <c r="B312" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C312" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E312" s="5" t="s">
         <v>59</v>
@@ -8303,27 +8316,27 @@
         <v>111</v>
       </c>
       <c r="B313" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C313" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E313" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="315" spans="1:6">
-      <c r="A315" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B315" s="5">
-        <v>101</v>
-      </c>
-      <c r="C315" s="5">
-        <v>101</v>
-      </c>
-      <c r="F315" s="5" t="s">
-        <v>65</v>
+    <row r="314" spans="1:6">
+      <c r="A314" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B314" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C314" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E314" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="316" spans="1:6">
@@ -8331,13 +8344,13 @@
         <v>114</v>
       </c>
       <c r="B316" s="5">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C316" s="5">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F316" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="317" spans="1:6">
@@ -8345,13 +8358,13 @@
         <v>114</v>
       </c>
       <c r="B317" s="5">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C317" s="5">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F317" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="318" spans="1:6">
@@ -8359,13 +8372,13 @@
         <v>114</v>
       </c>
       <c r="B318" s="5">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C318" s="5">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F318" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="319" spans="1:6">
@@ -8373,13 +8386,13 @@
         <v>114</v>
       </c>
       <c r="B319" s="5">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C319" s="5">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F319" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="320" spans="1:6">
@@ -8387,13 +8400,13 @@
         <v>114</v>
       </c>
       <c r="B320" s="5">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C320" s="5">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F320" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="321" spans="1:6">
@@ -8401,13 +8414,13 @@
         <v>114</v>
       </c>
       <c r="B321" s="5">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C321" s="5">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F321" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="322" spans="1:6">
@@ -8415,13 +8428,13 @@
         <v>114</v>
       </c>
       <c r="B322" s="5">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C322" s="5">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F322" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="323" spans="1:6">
@@ -8429,13 +8442,13 @@
         <v>114</v>
       </c>
       <c r="B323" s="5">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C323" s="5">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F323" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="324" spans="1:6">
@@ -8443,13 +8456,13 @@
         <v>114</v>
       </c>
       <c r="B324" s="5">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C324" s="5">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F324" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="325" spans="1:6">
@@ -8457,13 +8470,13 @@
         <v>114</v>
       </c>
       <c r="B325" s="5">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C325" s="5">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F325" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="326" spans="1:6">
@@ -8471,13 +8484,13 @@
         <v>114</v>
       </c>
       <c r="B326" s="5">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C326" s="5">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F326" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="327" spans="1:6">
@@ -8485,13 +8498,13 @@
         <v>114</v>
       </c>
       <c r="B327" s="5">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C327" s="5">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F327" s="5" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
     </row>
     <row r="328" spans="1:6">
@@ -8499,13 +8512,13 @@
         <v>114</v>
       </c>
       <c r="B328" s="5">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C328" s="5">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F328" s="5" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
     </row>
     <row r="329" spans="1:6">
@@ -8513,13 +8526,13 @@
         <v>114</v>
       </c>
       <c r="B329" s="5">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C329" s="5">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F329" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="330" spans="1:6">
@@ -8527,13 +8540,13 @@
         <v>114</v>
       </c>
       <c r="B330" s="5">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C330" s="5">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F330" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="331" spans="1:6">
@@ -8541,13 +8554,13 @@
         <v>114</v>
       </c>
       <c r="B331" s="5">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C331" s="5">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F331" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="332" spans="1:6">
@@ -8555,13 +8568,13 @@
         <v>114</v>
       </c>
       <c r="B332" s="5">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C332" s="5">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F332" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="333" spans="1:6">
@@ -8569,13 +8582,13 @@
         <v>114</v>
       </c>
       <c r="B333" s="5">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C333" s="5">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F333" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="334" spans="1:6">
@@ -8583,13 +8596,13 @@
         <v>114</v>
       </c>
       <c r="B334" s="5">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C334" s="5">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F334" s="5" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
     </row>
     <row r="335" spans="1:6">
@@ -8597,13 +8610,13 @@
         <v>114</v>
       </c>
       <c r="B335" s="5">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C335" s="5">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F335" s="5" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
     </row>
     <row r="336" spans="1:6">
@@ -8611,13 +8624,13 @@
         <v>114</v>
       </c>
       <c r="B336" s="5">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C336" s="5">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F336" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="337" spans="1:6">
@@ -8625,13 +8638,13 @@
         <v>114</v>
       </c>
       <c r="B337" s="5">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C337" s="5">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F337" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="338" spans="1:6">
@@ -8639,13 +8652,13 @@
         <v>114</v>
       </c>
       <c r="B338" s="5">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C338" s="5">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F338" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="339" spans="1:6">
@@ -8653,13 +8666,13 @@
         <v>114</v>
       </c>
       <c r="B339" s="5">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C339" s="5">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F339" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="340" spans="1:6">
@@ -8667,13 +8680,13 @@
         <v>114</v>
       </c>
       <c r="B340" s="5">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C340" s="5">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F340" s="5" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
     </row>
     <row r="341" spans="1:6">
@@ -8681,13 +8694,13 @@
         <v>114</v>
       </c>
       <c r="B341" s="5">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C341" s="5">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F341" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="342" spans="1:6">
@@ -8695,13 +8708,13 @@
         <v>114</v>
       </c>
       <c r="B342" s="5">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C342" s="5">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F342" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="343" spans="1:6">
@@ -8709,13 +8722,13 @@
         <v>114</v>
       </c>
       <c r="B343" s="5">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C343" s="5">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F343" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="344" spans="1:6">
@@ -8723,13 +8736,13 @@
         <v>114</v>
       </c>
       <c r="B344" s="5">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C344" s="5">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F344" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="345" spans="1:6">
@@ -8737,13 +8750,13 @@
         <v>114</v>
       </c>
       <c r="B345" s="5">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C345" s="5">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F345" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="346" spans="1:6">
@@ -8751,13 +8764,13 @@
         <v>114</v>
       </c>
       <c r="B346" s="5">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C346" s="5">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F346" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="347" spans="1:6">
@@ -8765,13 +8778,13 @@
         <v>114</v>
       </c>
       <c r="B347" s="5">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C347" s="5">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F347" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="348" spans="1:6">
@@ -8779,13 +8792,13 @@
         <v>114</v>
       </c>
       <c r="B348" s="5">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C348" s="5">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F348" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="349" spans="1:6">
@@ -8793,13 +8806,13 @@
         <v>114</v>
       </c>
       <c r="B349" s="5">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C349" s="5">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F349" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="350" spans="1:6">
@@ -8807,13 +8820,13 @@
         <v>114</v>
       </c>
       <c r="B350" s="5">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C350" s="5">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F350" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="351" spans="1:6">
@@ -8821,13 +8834,13 @@
         <v>114</v>
       </c>
       <c r="B351" s="5">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C351" s="5">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F351" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="352" spans="1:6">
@@ -8835,13 +8848,13 @@
         <v>114</v>
       </c>
       <c r="B352" s="5">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C352" s="5">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F352" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="353" spans="1:6">
@@ -8849,13 +8862,13 @@
         <v>114</v>
       </c>
       <c r="B353" s="5">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C353" s="5">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F353" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="354" spans="1:6">
@@ -8863,13 +8876,13 @@
         <v>114</v>
       </c>
       <c r="B354" s="5">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C354" s="5">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F354" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="355" spans="1:6">
@@ -8877,13 +8890,13 @@
         <v>114</v>
       </c>
       <c r="B355" s="5">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C355" s="5">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F355" s="5" t="s">
-        <v>62</v>
+        <v>101</v>
       </c>
     </row>
     <row r="356" spans="1:6">
@@ -8891,13 +8904,13 @@
         <v>114</v>
       </c>
       <c r="B356" s="5">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C356" s="5">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F356" s="5" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
     </row>
     <row r="357" spans="1:6">
@@ -8905,13 +8918,13 @@
         <v>114</v>
       </c>
       <c r="B357" s="5">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C357" s="5">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F357" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="358" spans="1:6">
@@ -8919,13 +8932,13 @@
         <v>114</v>
       </c>
       <c r="B358" s="5">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C358" s="5">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F358" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="359" spans="1:6">
@@ -8933,12 +8946,26 @@
         <v>114</v>
       </c>
       <c r="B359" s="5">
+        <v>144</v>
+      </c>
+      <c r="C359" s="5">
+        <v>144</v>
+      </c>
+      <c r="F359" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="360" spans="1:6">
+      <c r="A360" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B360" s="5">
         <v>145</v>
       </c>
-      <c r="C359" s="5">
+      <c r="C360" s="5">
         <v>145</v>
       </c>
-      <c r="F359" s="5" t="s">
+      <c r="F360" s="5" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>